<commit_message>
Tasks for block 1 complete
Block 1 outlined with detailed tasks. See document:
Tasks Tracking Block 1 docx

going to create the outline of the block 2 and make a visual
representation of the project plan.
</commit_message>
<xml_diff>
--- a/Administrative/Tasks/Tasks.xlsx
+++ b/Administrative/Tasks/Tasks.xlsx
@@ -468,7 +468,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -578,11 +577,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="285103464"/>
-        <c:axId val="285104248"/>
+        <c:axId val="239310456"/>
+        <c:axId val="239319080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="285103464"/>
+        <c:axId val="239310456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +624,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285104248"/>
+        <c:crossAx val="239319080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -633,7 +632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="285104248"/>
+        <c:axId val="239319080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +683,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285103464"/>
+        <c:crossAx val="239310456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C10:C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1638,7 @@
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1699,7 +1698,7 @@
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1739,7 +1738,7 @@
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1762,7 +1761,7 @@
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1776,13 +1775,13 @@
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1796,13 +1795,13 @@
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1816,11 +1815,11 @@
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1831,18 +1830,18 @@
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1850,7 +1849,7 @@
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1858,7 +1857,7 @@
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1866,7 +1865,7 @@
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>